<commit_message>
Interim version containing scoring controller and viewing supported in client controller (as well as joining)
</commit_message>
<xml_diff>
--- a/Contract Whist Scorecard/View flow host.xlsx
+++ b/Contract Whist Scorecard/View flow host.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcshearer/Documents/Xcode projects/Contract Whist Scorecard/Contract Whist Scorecard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7900701F-76D0-3B45-992C-5168DBDEDC84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F97C5612-138F-6340-80A4-8E2441876ECA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43220" yWindow="3060" windowWidth="28040" windowHeight="17440" xr2:uid="{8051CE0C-E72C-3C44-BBE4-205259BE231B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,9 +32,23 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Host</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Scoring</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -63,6 +77,20 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="48"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -84,11 +112,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -115,6 +147,82 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F936E107-73FF-C94D-91E3-2D433AAAAC87}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10121900" y="5518150"/>
+          <a:ext cx="1066800" cy="355600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800"/>
+            <a:t>Detail</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800" i="1" baseline="0"/>
+            <a:t>etc</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>698500</xdr:colOff>
       <xdr:row>12</xdr:row>
@@ -564,10 +672,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="accent4">
-            <a:lumMod val="40000"/>
-            <a:lumOff val="60000"/>
-          </a:schemeClr>
+          <a:srgbClr val="8FABDD"/>
         </a:solidFill>
       </xdr:spPr>
       <xdr:style>
@@ -590,12 +695,18 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr algn="ctr"/>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-GB" sz="2000"/>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>Game Summary</a:t>
           </a:r>
-          <a:endParaRPr lang="en-GB" sz="2400"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -634,10 +745,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="accent4">
-            <a:lumMod val="40000"/>
-            <a:lumOff val="60000"/>
-          </a:schemeClr>
+          <a:srgbClr val="8FABDD"/>
         </a:solidFill>
       </xdr:spPr>
       <xdr:style>
@@ -660,12 +768,18 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr algn="ctr"/>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-GB" sz="2000"/>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>Confirm</a:t>
           </a:r>
-          <a:endParaRPr lang="en-GB" sz="2400"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -704,10 +818,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="accent4">
-            <a:lumMod val="40000"/>
-            <a:lumOff val="60000"/>
-          </a:schemeClr>
+          <a:srgbClr val="8FABDD"/>
         </a:solidFill>
       </xdr:spPr>
       <xdr:style>
@@ -730,12 +841,18 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr algn="ctr"/>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-GB" sz="1800"/>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>Review</a:t>
           </a:r>
-          <a:endParaRPr lang="en-GB" sz="2000"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -774,9 +891,9 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="accent4">
-            <a:lumMod val="40000"/>
-            <a:lumOff val="60000"/>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
       </xdr:spPr>
@@ -800,16 +917,30 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr algn="ctr"/>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-GB" sz="2000"/>
+            <a:rPr lang="en-GB" sz="2000">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>Select</a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:pPr algn="ctr"/>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-GB" sz="2000"/>
+            <a:rPr lang="en-GB" sz="2000">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>Players</a:t>
           </a:r>
         </a:p>
@@ -850,10 +981,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="accent4">
-            <a:lumMod val="40000"/>
-            <a:lumOff val="60000"/>
-          </a:schemeClr>
+          <a:srgbClr val="8FABDD"/>
         </a:solidFill>
       </xdr:spPr>
       <xdr:style>
@@ -876,12 +1004,18 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr algn="ctr"/>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-GB" sz="2000"/>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>Location</a:t>
           </a:r>
-          <a:endParaRPr lang="en-GB" sz="2400"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -920,9 +1054,9 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="accent4">
-            <a:lumMod val="40000"/>
-            <a:lumOff val="60000"/>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
       </xdr:spPr>
@@ -946,12 +1080,18 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr algn="ctr"/>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-GB" sz="2000"/>
+            <a:rPr lang="en-GB" sz="2000">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>Override Settings</a:t>
           </a:r>
-          <a:endParaRPr lang="en-GB" sz="2400"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1239,13 +1379,13 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>804335</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>804335</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1256,14 +1396,11 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="16" idx="0"/>
-          <a:endCxn id="19" idx="2"/>
-        </xdr:cNvCxnSpPr>
+        <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="9059335" y="1765300"/>
+          <a:off x="9059335" y="1752600"/>
           <a:ext cx="0" cy="457200"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -1408,13 +1545,13 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>46568</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>46568</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1429,7 +1566,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="7476068" y="2679700"/>
+          <a:off x="7476068" y="2667000"/>
           <a:ext cx="0" cy="228600"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -1888,6 +2025,3776 @@
         </a:prstGeom>
         <a:ln w="38100">
           <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="Rectangle 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2933B46E-F7A9-4D40-9985-5994862240E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10071100" y="4241800"/>
+          <a:ext cx="1168400" cy="977900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="8FABDD"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>High</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Scores</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>567268</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Straight Arrow Connector 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F70CC6C2-423A-3D46-8033-6C5F4C5B1D09}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9647768" y="4197350"/>
+          <a:ext cx="423332" cy="349250"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="Straight Arrow Connector 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B620BFD-07EB-CF4E-8936-BE15D7A41A65}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="35" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10655300" y="5219700"/>
+          <a:ext cx="0" cy="355600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="Rectangle 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C884140-E070-C543-9E4E-BE256D4EF311}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="825500" y="10452100"/>
+          <a:ext cx="1168400" cy="977900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2400"/>
+            <a:t>Home </a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-GB" sz="2400"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2400"/>
+            <a:t>Screen</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>753534</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>270934</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="45" name="Rectangle 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C5CC177-E6DA-A346-BFB6-E80D37D9E4D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2404534" y="10452100"/>
+          <a:ext cx="1168400" cy="977900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2000"/>
+            <a:t>Game Preview</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="2400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>681568</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>198968</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="Rectangle 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{811F0A0F-69FF-584E-B962-683CA5B161BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3983568" y="10452100"/>
+          <a:ext cx="1168400" cy="977900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2000"/>
+            <a:t>Hand</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="2400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>613835</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>131235</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name="Rectangle 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F4C6832-5938-D844-BC26-7879619845A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5566835" y="9766300"/>
+          <a:ext cx="1168400" cy="977900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="8FABDD"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800"/>
+            <a:t>Scorepad</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="2000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>613835</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>131235</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="Rectangle 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A02EE4B9-15DE-0A4C-9EF8-2437B3244798}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5566835" y="11188700"/>
+          <a:ext cx="1168400" cy="977900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="8FABDD"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Game Summary</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>681568</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>198968</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="49" name="Rectangle 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{450C870D-5A18-9547-8ADF-EA3F2A3FD1EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3983568" y="9245600"/>
+          <a:ext cx="1168400" cy="977900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="8FABDD"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Confirm</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>613835</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>131235</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="Rectangle 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C6E05B7-BA6C-F643-B4C5-B12F68DF86CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5566835" y="8331200"/>
+          <a:ext cx="1168400" cy="977900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="8FABDD"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Review</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>745067</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="Straight Arrow Connector 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50F2B66F-A751-D348-838B-EDD43FE7CD5B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1981200" y="10941050"/>
+          <a:ext cx="414867" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="solid"/>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>694267</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="52" name="Straight Arrow Connector 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A6CBB42-5070-CE44-B7DB-D0EA27A4BEDA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3581400" y="10941050"/>
+          <a:ext cx="414867" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>198968</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>613835</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="53" name="Straight Arrow Connector 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97C583FE-210D-C242-9BB3-B2A8796E65D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="46" idx="3"/>
+          <a:endCxn id="47" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5151968" y="10255250"/>
+          <a:ext cx="414867" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>372535</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>372535</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="54" name="Straight Arrow Connector 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82643083-07F3-4F46-8E30-0BF899BD345A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6151035" y="9296400"/>
+          <a:ext cx="0" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>440268</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>440268</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="55" name="Straight Arrow Connector 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CEEDE89-AC1B-1248-A27A-8B3B1A3DA2EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4567768" y="10223500"/>
+          <a:ext cx="0" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>198968</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>613835</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="56" name="Straight Arrow Connector 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB0A4088-05CC-3E49-96D4-E95CB679F628}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="46" idx="3"/>
+          <a:endCxn id="48" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5151968" y="10941050"/>
+          <a:ext cx="414867" cy="736600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="57" name="Rectangle 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3D6A451-B94E-694E-BC78-0D05480E1DAE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7162800" y="9766300"/>
+          <a:ext cx="1168400" cy="977900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:alpha val="20000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+              <a:alpha val="20000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2400"/>
+            <a:t>Home </a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-GB" sz="2400"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2400"/>
+            <a:t>Screen</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>554567</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="58" name="Straight Arrow Connector 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A95CAAAE-6D6E-3E44-9865-5149C7A53054}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6743700" y="10255250"/>
+          <a:ext cx="414867" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>131235</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="59" name="Straight Arrow Connector 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6694722-4FA6-AB42-909F-834FCC445858}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="48" idx="3"/>
+          <a:endCxn id="57" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6735235" y="10744200"/>
+          <a:ext cx="1011765" cy="933450"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:headEnd type="none"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>613835</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>131235</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="60" name="Rectangle 59">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9842F39-9971-E048-BE62-54F0A2F3F2A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5566835" y="12573000"/>
+          <a:ext cx="1168400" cy="977900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:alpha val="20000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+              <a:alpha val="20000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2400"/>
+            <a:t>Hand</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400"/>
+            <a:t>Next Game</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="2000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61" name="Rectangle 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CECC1086-E0B7-4042-9EAD-DEF71521145F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7162800" y="11785600"/>
+          <a:ext cx="1168400" cy="977900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="8FABDD"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>High</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Scores</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>135468</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="62" name="Straight Arrow Connector 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96326CED-12BD-884F-BDCC-D14761C18051}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6739468" y="11728450"/>
+          <a:ext cx="423332" cy="349250"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="63" name="Straight Arrow Connector 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D821DBDF-063A-CB4B-8D76-E594B4A4DF17}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6146800" y="12153900"/>
+          <a:ext cx="0" cy="406400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="64" name="Straight Arrow Connector 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF49E85A-1EA9-3541-861D-CC20373FFDAB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6146800" y="10756900"/>
+          <a:ext cx="0" cy="444500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="65" name="TextBox 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC069083-4901-DA4D-BBDE-D7736DACBF1A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7226300" y="13061950"/>
+          <a:ext cx="1066800" cy="355600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800"/>
+            <a:t>Detail</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800" i="1" baseline="0"/>
+            <a:t>etc</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="66" name="Straight Arrow Connector 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1920F3B5-7BF0-1E4E-AD7B-AB0D5D4FF236}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7759700" y="12763500"/>
+          <a:ext cx="0" cy="355600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="93" name="Arc 92">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D7852ED-3B76-A143-8846-EB10DC91443C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="5092700" y="16637000"/>
+          <a:ext cx="2146300" cy="1625600"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 11677133"/>
+            <a:gd name="adj2" fmla="val 20753166"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="94" name="Rectangle 93">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69079F15-0876-3B41-8CC4-6B335038E229}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="825500" y="16954500"/>
+          <a:ext cx="1168400" cy="977900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2400"/>
+            <a:t>Home </a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-GB" sz="2400"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2400"/>
+            <a:t>Screen</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>757767</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>275167</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="95" name="Rectangle 94">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1DAD267-831B-4B45-BE09-07535CA42755}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2408767" y="16954500"/>
+          <a:ext cx="1168400" cy="977900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2000"/>
+            <a:t>Selection</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="2400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>690034</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>207434</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="96" name="Rectangle 95">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E83ABCE-E118-244D-91AD-E1133F47646D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3992034" y="16954500"/>
+          <a:ext cx="1168400" cy="977900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2000"/>
+            <a:t>Game Preview</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="2400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>757767</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>275167</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="100" name="Rectangle 99">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7E785DC-F454-6A4D-A784-1DAE4D6B7008}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2408767" y="15748000"/>
+          <a:ext cx="1168400" cy="977900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2000">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Select</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2000">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Players</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>622301</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>139701</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="101" name="Rectangle 100">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03420218-496E-5048-A8A6-E9DB98903BAA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5575301" y="16954500"/>
+          <a:ext cx="1168400" cy="977900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="8FABDD"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Location</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>690034</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>207434</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="102" name="Rectangle 101">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BA74451-8DBA-6640-AB83-16F356273F0D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3992034" y="18161000"/>
+          <a:ext cx="1168400" cy="977900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2000">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Override Settings</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>757767</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="103" name="Straight Arrow Connector 102">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{274C5E01-AFE3-584A-87AB-D3F8324DC77F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1993900" y="17443450"/>
+          <a:ext cx="414867" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100" cmpd="sng">
+          <a:prstDash val="solid"/>
+          <a:headEnd type="triangle" w="sm" len="med"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>681567</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="104" name="Straight Arrow Connector 103">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DAB1C9B-ACDD-3949-BAC0-995BFE80B1E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3568700" y="17443450"/>
+          <a:ext cx="414867" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="solid"/>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>618067</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="105" name="Straight Arrow Connector 104">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03C4F23A-19D0-8E4A-9A4C-99D39887A6A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5156200" y="17443450"/>
+          <a:ext cx="414867" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>139701</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="106" name="Straight Arrow Connector 105">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D8445D0-EBE1-B24C-9532-22FFF4B9B4AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="101" idx="3"/>
+          <a:endCxn id="128" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6743701" y="17443450"/>
+          <a:ext cx="457199" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>448734</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>448734</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="108" name="Straight Arrow Connector 107">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8073F9C7-B56E-B140-B4DE-65A92B28667C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4576234" y="17932400"/>
+          <a:ext cx="0" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>554567</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>554567</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="110" name="Straight Arrow Connector 109">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8389812-4802-F643-A949-2BE9B5074098}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3031067" y="16725900"/>
+          <a:ext cx="0" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="118" name="Rectangle 117">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6404A76-B4CC-3249-B293-C8539CE49C4C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7200900" y="15405100"/>
+          <a:ext cx="1168400" cy="977900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="8FABDD"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Round</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Summary</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>524932</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>766232</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="127" name="TextBox 126">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78A4A189-9976-364F-ACB6-FD21FFD1AB29}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10430932" y="19564350"/>
+          <a:ext cx="1066800" cy="355600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800"/>
+            <a:t>Detail</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800" i="1" baseline="0"/>
+            <a:t>etc</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="128" name="Rectangle 127">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A40E5C42-19ED-4F42-9479-5E762A6729B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7200900" y="16954500"/>
+          <a:ext cx="1168400" cy="977900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2000"/>
+            <a:t>Entry</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="2400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>529167</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>46567</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="129" name="Rectangle 128">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC5B4B59-D823-824D-B731-BB32799B89C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8784167" y="16268700"/>
+          <a:ext cx="1168400" cy="977900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="8FABDD"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800"/>
+            <a:t>Scorepad</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="2000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>529167</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>46567</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="130" name="Rectangle 129">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A3B408B-A715-8445-A39B-507CC643C1AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8784167" y="17691100"/>
+          <a:ext cx="1168400" cy="977900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="8FABDD"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Game Summary</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>529167</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="132" name="Straight Arrow Connector 131">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19BA3AA1-BC16-344E-9652-54BB7C36BB58}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="128" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8369300" y="16757650"/>
+          <a:ext cx="414867" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="133" name="Straight Arrow Connector 132">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5398EABB-79C3-2C48-AC0C-BD47D58AA563}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="128" idx="0"/>
+          <a:endCxn id="118" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7785100" y="16383000"/>
+          <a:ext cx="0" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>287867</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>287867</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="134" name="Straight Arrow Connector 133">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{543493C7-643A-C843-8797-BB5D6AA823F1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="130" idx="0"/>
+          <a:endCxn id="129" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9368367" y="17246600"/>
+          <a:ext cx="0" cy="444500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>529167</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="135" name="Straight Arrow Connector 134">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A2315E3-36DE-584F-835E-3C6E3F3F8C2C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="128" idx="3"/>
+          <a:endCxn id="130" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8369300" y="17443450"/>
+          <a:ext cx="414867" cy="736600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>474132</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>817032</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="136" name="Rectangle 135">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C17F3FA-A86E-C24F-9497-C31EF01E79CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10380132" y="16268700"/>
+          <a:ext cx="1168400" cy="977900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:alpha val="20000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+              <a:alpha val="20000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2400"/>
+            <a:t>Home </a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-GB" sz="2400"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2400"/>
+            <a:t>Screen</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>55032</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>469899</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="137" name="Straight Arrow Connector 136">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA576B6D-010C-634D-8C23-73AFBF7FF7F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9961032" y="16757650"/>
+          <a:ext cx="414867" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>46567</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>232832</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="138" name="Straight Arrow Connector 137">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE6AC531-7431-764E-97E9-B582DE9A7DC1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="130" idx="3"/>
+          <a:endCxn id="136" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9952567" y="17246600"/>
+          <a:ext cx="1011765" cy="933450"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:headEnd type="none"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>529167</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>46567</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="139" name="Rectangle 138">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E05A503-16FD-E04A-94CA-9B2E4C5BBCDF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8784167" y="19075400"/>
+          <a:ext cx="1168400" cy="977900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:alpha val="20000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+              <a:alpha val="20000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2400"/>
+            <a:t>Entry</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400"/>
+            <a:t>Next Game</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="2000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>287867</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>287867</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="140" name="Straight Arrow Connector 139">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5B70FAA-1D5F-754B-B38D-D63A110EE62B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="130" idx="2"/>
+          <a:endCxn id="139" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9368367" y="18669000"/>
+          <a:ext cx="0" cy="406400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>474132</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>817032</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="141" name="Rectangle 140">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{338ACA19-3383-774D-9094-E1EE8112D51B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10380132" y="18288000"/>
+          <a:ext cx="1168400" cy="977900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="8FABDD"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>High</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Scores</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>232832</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>232832</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="142" name="Straight Arrow Connector 141">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C2ADFCC-E8A4-1841-BD48-2D88A45DBA24}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="141" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10964332" y="19265900"/>
+          <a:ext cx="0" cy="355600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>474132</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="145" name="Straight Arrow Connector 144">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8E4D1C6-1E50-3D40-B713-6012122F1302}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9956800" y="18440400"/>
+          <a:ext cx="423332" cy="349250"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="156" name="Straight Arrow Connector 155">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{750726D3-DEF2-964F-87D2-F4C698A39220}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="118" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8369300" y="15894050"/>
+          <a:ext cx="419100" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:headEnd type="triangle"/>
           <a:tailEnd type="triangle"/>
         </a:ln>
       </xdr:spPr>
@@ -2208,23 +6115,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A066CC22-D0C1-C54E-9C91-CCE15E896E7F}">
-  <dimension ref="E13:N26"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:N75"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+      <selection activeCell="E100" sqref="E100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="13" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="M13" s="3"/>
       <c r="N13" s="2"/>
     </row>
     <row r="26" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E26" s="1"/>
     </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="64" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J64" s="5"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73" s="4"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" s="4"/>
+      <c r="B74" s="4"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="4"/>
+    </row>
+    <row r="75" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E3"/>
+    <mergeCell ref="A35:E37"/>
+    <mergeCell ref="A73:E75"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="49" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>